<commit_message>
Updating figures to Arial.
</commit_message>
<xml_diff>
--- a/Optimization case study - JoH/ressources/analogues nb.xlsx
+++ b/Optimization case study - JoH/ressources/analogues nb.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="results" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -3209,11 +3209,11 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -3256,23 +3256,15 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-CH">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="fr-CH"/>
                   <a:t>Number of analogues</a:t>
                 </a:r>
               </a:p>
@@ -3301,14 +3293,11 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="de-DE"/>
@@ -3333,11 +3322,11 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -3373,11 +3362,11 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="de-DE"/>
@@ -3408,7 +3397,13 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -25983,7 +25978,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM17 IM30">
+  <conditionalFormatting sqref="IM30 IM17">
     <cfRule type="colorScale" priority="385">
       <colorScale>
         <cfvo type="min"/>
@@ -25995,7 +25990,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN17 IN30">
+  <conditionalFormatting sqref="IN30 IN17">
     <cfRule type="colorScale" priority="387">
       <colorScale>
         <cfvo type="min"/>
@@ -26007,7 +26002,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM18 IM31">
+  <conditionalFormatting sqref="IM31 IM18">
     <cfRule type="colorScale" priority="396">
       <colorScale>
         <cfvo type="min"/>
@@ -26019,7 +26014,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN18 IN31">
+  <conditionalFormatting sqref="IN31 IN18">
     <cfRule type="colorScale" priority="398">
       <colorScale>
         <cfvo type="min"/>
@@ -26031,7 +26026,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM19 IM32">
+  <conditionalFormatting sqref="IM32 IM19">
     <cfRule type="colorScale" priority="407">
       <colorScale>
         <cfvo type="min"/>
@@ -26043,7 +26038,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN19 IN32">
+  <conditionalFormatting sqref="IN32 IN19">
     <cfRule type="colorScale" priority="409">
       <colorScale>
         <cfvo type="min"/>
@@ -26055,7 +26050,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM20 IM33">
+  <conditionalFormatting sqref="IM33 IM20">
     <cfRule type="colorScale" priority="418">
       <colorScale>
         <cfvo type="min"/>
@@ -26067,7 +26062,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN20 IN33">
+  <conditionalFormatting sqref="IN33 IN20">
     <cfRule type="colorScale" priority="420">
       <colorScale>
         <cfvo type="min"/>
@@ -26079,7 +26074,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM21 IM34">
+  <conditionalFormatting sqref="IM34 IM21">
     <cfRule type="colorScale" priority="429">
       <colorScale>
         <cfvo type="min"/>
@@ -26091,7 +26086,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN21 IN34">
+  <conditionalFormatting sqref="IN34 IN21">
     <cfRule type="colorScale" priority="431">
       <colorScale>
         <cfvo type="min"/>
@@ -26103,7 +26098,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM35 IM22">
+  <conditionalFormatting sqref="IM22 IM35">
     <cfRule type="colorScale" priority="440">
       <colorScale>
         <cfvo type="min"/>
@@ -26115,7 +26110,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN35 IN22">
+  <conditionalFormatting sqref="IN22 IN35">
     <cfRule type="colorScale" priority="442">
       <colorScale>
         <cfvo type="min"/>
@@ -26127,7 +26122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM36 IM23">
+  <conditionalFormatting sqref="IM23 IM36">
     <cfRule type="colorScale" priority="451">
       <colorScale>
         <cfvo type="min"/>
@@ -26139,7 +26134,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN36 IN23">
+  <conditionalFormatting sqref="IN23 IN36">
     <cfRule type="colorScale" priority="453">
       <colorScale>
         <cfvo type="min"/>
@@ -26151,7 +26146,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM37 IM24">
+  <conditionalFormatting sqref="IM24 IM37">
     <cfRule type="colorScale" priority="462">
       <colorScale>
         <cfvo type="min"/>
@@ -26163,7 +26158,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN37 IN24">
+  <conditionalFormatting sqref="IN24 IN37">
     <cfRule type="colorScale" priority="464">
       <colorScale>
         <cfvo type="min"/>
@@ -26175,7 +26170,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IM38 IM25">
+  <conditionalFormatting sqref="IM25 IM38">
     <cfRule type="colorScale" priority="473">
       <colorScale>
         <cfvo type="min"/>
@@ -26187,7 +26182,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IN38 IN25">
+  <conditionalFormatting sqref="IN25 IN38">
     <cfRule type="colorScale" priority="475">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>